<commit_message>
Drop-in user as owner/member
</commit_message>
<xml_diff>
--- a/Deployment/Power Apps/ClassroomDropin.xlsx
+++ b/Deployment/Power Apps/ClassroomDropin.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="184">
   <si>
     <t>Locale</t>
   </si>
@@ -549,6 +549,43 @@
   </si>
   <si>
     <t>is ready. They have also been sent a confirmation message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bonjour,</t>
+  </si>
+  <si>
+    <t>Nouveau drop-in</t>
+  </si>
+  <si>
+    <t>Visiter une classe virtuelle</t>
+  </si>
+  <si>
+    <t>Drop-ins programmés</t>
+  </si>
+  <si>
+    <t>Afficher les détails ou prolonger la durée</t>
+  </si>
+  <si>
+    <t>en-ES</t>
+  </si>
+  <si>
+    <t>OwnerOrMemberLbl</t>
+  </si>
+  <si>
+    <t>Dropping the user as :</t>
+  </si>
+  <si>
+    <t>OwnerLbl</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>MemberLbl</t>
+  </si>
+  <si>
+    <t>Member</t>
   </si>
 </sst>
 </file>
@@ -613,9 +650,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="colTranslation" displayName="colTranslation" ref="A1:CK10" totalsRowShown="0">
-  <autoFilter ref="A1:CK10"/>
-  <tableColumns count="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="colTranslation" displayName="colTranslation" ref="A1:CN10" totalsRowShown="0">
+  <autoFilter ref="A1:CN10"/>
+  <tableColumns count="92">
     <tableColumn id="1" name="Locale"/>
     <tableColumn id="2" name="IsSupported"/>
     <tableColumn id="3" name="WelcomeMessage"/>
@@ -705,6 +742,9 @@
     <tableColumn id="87" name="OpenClassroomDropInAppBtnTxt"/>
     <tableColumn id="88" name="OpenTxt"/>
     <tableColumn id="89" name="MessageTxt"/>
+    <tableColumn id="90" name="OwnerOrMemberLbl"/>
+    <tableColumn id="91" name="OwnerLbl"/>
+    <tableColumn id="92" name="MemberLbl"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -973,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK2"/>
+  <dimension ref="A1:CN3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BV2" sqref="BV2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="CI19" sqref="CI19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,7 +1070,7 @@
     <col min="52" max="52" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:92" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1298,8 +1338,17 @@
       <c r="CK1" t="s">
         <v>168</v>
       </c>
+      <c r="CL1" t="s">
+        <v>178</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>180</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>182</v>
+      </c>
     </row>
-    <row r="2" spans="1:89" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:92" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1566,6 +1615,38 @@
       </c>
       <c r="CK2" t="s">
         <v>169</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>179</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>181</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:92" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for removing premium Power Automate license.
</commit_message>
<xml_diff>
--- a/Deployment/Power Apps/ClassroomDropin.xlsx
+++ b/Deployment/Power Apps/ClassroomDropin.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="186">
   <si>
     <t>Locale</t>
   </si>
@@ -549,6 +549,49 @@
   </si>
   <si>
     <t>is ready. They have also been sent a confirmation message.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bonjour,</t>
+  </si>
+  <si>
+    <t>Nouveau drop-in</t>
+  </si>
+  <si>
+    <t>Visiter une classe virtuelle</t>
+  </si>
+  <si>
+    <t>Drop-ins programmés</t>
+  </si>
+  <si>
+    <t>Afficher les détails ou prolonger la durée</t>
+  </si>
+  <si>
+    <t>en-ES</t>
+  </si>
+  <si>
+    <t>OwnerOrMemberLbl</t>
+  </si>
+  <si>
+    <t>Dropping the user as :</t>
+  </si>
+  <si>
+    <t>OwnerLbl</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>MemberLbl</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>NoPermissionLbl</t>
+  </si>
+  <si>
+    <t>Uh oh! Looks like you don't have permissions to use this app. Please contact IT/support.</t>
   </si>
 </sst>
 </file>
@@ -613,9 +656,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="colTranslation" displayName="colTranslation" ref="A1:CK10" totalsRowShown="0">
-  <autoFilter ref="A1:CK10"/>
-  <tableColumns count="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="colTranslation" displayName="colTranslation" ref="A1:CO10" totalsRowShown="0">
+  <autoFilter ref="A1:CO10"/>
+  <tableColumns count="93">
     <tableColumn id="1" name="Locale"/>
     <tableColumn id="2" name="IsSupported"/>
     <tableColumn id="3" name="WelcomeMessage"/>
@@ -705,6 +748,10 @@
     <tableColumn id="87" name="OpenClassroomDropInAppBtnTxt"/>
     <tableColumn id="88" name="OpenTxt"/>
     <tableColumn id="89" name="MessageTxt"/>
+    <tableColumn id="90" name="OwnerOrMemberLbl"/>
+    <tableColumn id="91" name="OwnerLbl"/>
+    <tableColumn id="92" name="MemberLbl"/>
+    <tableColumn id="93" name="NoPermissionLbl"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -973,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK2"/>
+  <dimension ref="A1:CO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BV2" sqref="BV2"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <selection activeCell="CO1" sqref="CO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1030,7 +1077,7 @@
     <col min="52" max="52" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:93" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1298,8 +1345,20 @@
       <c r="CK1" t="s">
         <v>168</v>
       </c>
+      <c r="CL1" t="s">
+        <v>178</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>180</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>182</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>184</v>
+      </c>
     </row>
-    <row r="2" spans="1:89" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:93" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1566,6 +1625,41 @@
       </c>
       <c r="CK2" t="s">
         <v>169</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>179</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>181</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>183</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:93" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>